<commit_message>
new chnges in ui/ux
</commit_message>
<xml_diff>
--- a/media/user_data.xlsx
+++ b/media/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,9 +476,24 @@
           <t xml:space="preserve">first one </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>35</t>
+      <c r="C3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sudhanshu </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kumar </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>25</t>
         </is>
       </c>
     </row>

</xml_diff>